<commit_message>
Added new page for IPA module and 1 script is added for IPA module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -39,13 +39,13 @@
     <t>SKIP</t>
   </si>
   <si>
-    <t>Ipa001</t>
-  </si>
-  <si>
     <t>OBT</t>
   </si>
   <si>
     <t>Login to IPA App</t>
+  </si>
+  <si>
+    <t>IPA001</t>
   </si>
 </sst>
 </file>
@@ -440,13 +440,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added test cases in IPA module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>TCID</t>
   </si>
@@ -42,10 +42,16 @@
     <t>OBT</t>
   </si>
   <si>
-    <t>Login to IPA App</t>
-  </si>
-  <si>
     <t>IPA001</t>
+  </si>
+  <si>
+    <t>IPA111</t>
+  </si>
+  <si>
+    <t>Save the company search data and rerun the saved data</t>
+  </si>
+  <si>
+    <t>Save the technology search data and rerun the saved data</t>
   </si>
 </sst>
 </file>
@@ -108,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,13 +447,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -454,6 +461,19 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added script in ipa.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>TCID</t>
   </si>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -472,8 +472,12 @@
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Checking in the my scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -52,12 +52,31 @@
   </si>
   <si>
     <t>Save the technology search data and rerun the saved data</t>
+  </si>
+  <si>
+    <t>NEON-291||NEON-400||NEON-438||NEON-574</t>
+  </si>
+  <si>
+    <t>User must be able to form a Technology Search||User must be able to return to the app landing page via the App header to start a new search||Option on the IPA App header to allow the user to return to the app landing page||User must be able to form a Company Search</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>IPA012</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -414,18 +433,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="63" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="63.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -456,7 +476,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -473,10 +493,27 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added New script for IPA Landing Page
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>TCID</t>
   </si>
@@ -60,9 +60,6 @@
     <t>User must be able to form a Technology Search||User must be able to return to the app landing page via the App header to start a new search||Option on the IPA App header to allow the user to return to the app landing page||User must be able to form a Company Search</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>IPA012</t>
   </si>
   <si>
@@ -70,14 +67,31 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>OPQA-4176||OPQA-4178||OPQA-4179||OPQA-4182||OPQA-4187||OPQA-4189 </t>
+  </si>
+  <si>
+    <t>IPA0001</t>
+  </si>
+  <si>
+    <t>Verify that, accessing of the URL  takes the user to DRA application Landing page || Verify that DRA Landing page, displays application branding and logo || Verify that DRA Landing page, contains feature promotion and iconography in the marketing section || Verify that DRA Landing page, displays link to privacy statement and terms of use. || verify that DRA Landing page, displays the message and email id on the DRA landing page "Having trouble with sign-in? please contact DRA_support@thomsonreuters.com "||</t>
+  </si>
+  <si>
+    <t>OPQA-4249 ||OPQA-4247 ||OPQA-4238</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that when linking a social with a matching email, if the user click [X] cross mark on the screen then he will be taken back to the DRA Login page. || Verify that text on the modal "Already have an account? .. ||Verify that when linking a social with a matching email, if the user clicks outside the Linking modal on the screen then nothing should happens</t>
+  </si>
+  <si>
+    <t>IPA0002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,18 +147,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -223,6 +245,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -257,6 +280,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,23 +456,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="63.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="63" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -476,13 +500,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -493,15 +517,15 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -513,33 +537,66 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Script - IPA
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>TCID</t>
   </si>
@@ -108,6 +103,24 @@
   </si>
   <si>
     <t>From DRA\IPA , Verify that system is able to merge Activated STeAM account and Activated Facebook account and after merge verify STeAM TRUID is change||Verify that If a user signs into DRA \IPA with a STeAM account that has a social account linked, the user should still see their linked social accounts on their account settings page.</t>
+  </si>
+  <si>
+    <t>OPQA-4241||OPQA-4245</t>
+  </si>
+  <si>
+    <t>Verify that user can skip the linking by clicking on "Not now button" on the modal "Already have an account? .. || Verify that once the user skips linking then user will not be prompted to link again.</t>
+  </si>
+  <si>
+    <t>IPA0003</t>
+  </si>
+  <si>
+    <t>IPA0004</t>
+  </si>
+  <si>
+    <t>Verify that error message " Incorrect password. Please try again."should be displayed when user enters incorrect password for existing steam account.|| Verify that when user's account is locked due to 10 invalid authentications of existing password,user becomes locked, the user is signed out</t>
+  </si>
+  <si>
+    <t>OPQA-4221 || OPQA-4225</t>
   </si>
 </sst>
 </file>
@@ -243,7 +256,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,7 +291,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" activeCellId="1" sqref="C14 B8"/>
+      <selection activeCell="A10" sqref="A10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,9 +643,40 @@
       </c>
       <c r="E8" s="4"/>
     </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>
+    <hyperlink ref="B10" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
IPA New Script for Change Password in Account settings
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>TCID</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>OPQA-4221 || OPQA-4225</t>
+  </si>
+  <si>
+    <t>OPQA-4223 || OPQA-4224</t>
+  </si>
+  <si>
+    <t>Verify that error message " New password should not match current password" should be displayed when user enters the current password in change password field.|| Verify that error message"New password should not match previous 4 passwords" should be displayed when user enters password in change password field which is matching with the previous 4 passwords.</t>
+  </si>
+  <si>
+    <t>IPA0005</t>
   </si>
 </sst>
 </file>
@@ -500,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,10 +682,26 @@
       </c>
       <c r="E10" s="6"/>
     </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>
     <hyperlink ref="B10" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
+    <hyperlink ref="B11" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4223"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new test case is added to IPA module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -68,9 +63,6 @@
     <t>IPA012</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>FAIL</t>
   </si>
   <si>
@@ -153,13 +145,16 @@
   </si>
   <si>
     <t>IPA052</t>
+  </si>
+  <si>
+    <t>IPA112</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,10 +315,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,7 +349,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -531,14 +524,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -547,7 +540,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -575,13 +568,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -592,13 +585,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -612,143 +605,160 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="120">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="90">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="75">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="90">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="C9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="75">
+      <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="90">
+      <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="C13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4"/>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -761,24 +771,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New test cases is added to IPA mpdule and new page is created for pages folder
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="6210"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
   <si>
     <t>TCID</t>
   </si>
@@ -230,13 +230,16 @@
   </si>
   <si>
     <t>Verify that user should not be allowed to sign-in to DRA \IPA when user account is locked ||Verify that user should not be allowed to sign-in to DRA \IPA when user account is evicted/Suspended .</t>
+  </si>
+  <si>
+    <t>IPA113</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,7 +428,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -460,7 +462,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -636,14 +637,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -652,7 +653,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -686,7 +687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -703,7 +704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -720,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="120">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -735,7 +736,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="90">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -750,7 +751,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="75">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -765,7 +766,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="90">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -780,7 +781,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
@@ -795,7 +796,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="75">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
@@ -810,7 +811,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="90">
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
@@ -825,7 +826,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45">
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
@@ -840,7 +841,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -855,7 +856,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -872,7 +873,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="105">
       <c r="A15" s="6" t="s">
         <v>44</v>
       </c>
@@ -887,7 +888,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="120">
       <c r="A16" s="6" t="s">
         <v>45</v>
       </c>
@@ -902,7 +903,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -916,7 +917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -930,7 +931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="120">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -944,7 +945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="75">
       <c r="A20" s="5" t="s">
         <v>55</v>
       </c>
@@ -958,7 +959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="45">
       <c r="A21" s="5" t="s">
         <v>58</v>
       </c>
@@ -972,7 +973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="45">
       <c r="A22" s="5" t="s">
         <v>61</v>
       </c>
@@ -986,7 +987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="45">
       <c r="A23" s="5" t="s">
         <v>64</v>
       </c>
@@ -999,6 +1000,21 @@
       <c r="D23" s="5" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1011,24 +1027,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New test script added to IPA module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
   <si>
     <t>TCID</t>
   </si>
@@ -293,12 +293,14 @@
   <si>
     <t>IPA14</t>
   </si>
+  <si>
+    <t>IPA114</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -698,19 +700,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="63.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="63" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1163,6 +1165,21 @@
       <c r="E29" s="4" t="s">
         <v>75</v>
       </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
new test cases aree added to IPA module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
   <si>
     <t>TCID</t>
   </si>
@@ -298,6 +298,72 @@
   </si>
   <si>
     <t>User must be able to select to record on the result list to view its full content</t>
+  </si>
+  <si>
+    <t>IPA115</t>
+  </si>
+  <si>
+    <t>IPA02</t>
+  </si>
+  <si>
+    <t>OPQA-4402||OPQA-4403||OPQA-4404||OPQA-4405</t>
+  </si>
+  <si>
+    <t>Veify Technology competitors visualization</t>
+  </si>
+  <si>
+    <t>IPA03</t>
+  </si>
+  <si>
+    <t>OPQA-4397||OPQA-4398||OPQA-4400||OPQA-4401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Technology trending visualization </t>
+  </si>
+  <si>
+    <t>IPA04</t>
+  </si>
+  <si>
+    <t>OPQA-4412||OPQA-4413||OPQA-4415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Company Technology trending visualization </t>
+  </si>
+  <si>
+    <t>IPA05</t>
+  </si>
+  <si>
+    <t>OPQA-4425||OPQA-4423||OPQA-4421</t>
+  </si>
+  <si>
+    <t>Verify Company Key Information</t>
+  </si>
+  <si>
+    <t>IPA06</t>
+  </si>
+  <si>
+    <t>OPQA-4444||OPQA-4445||OPQA-4446</t>
+  </si>
+  <si>
+    <t>Verify Technology Key Information</t>
+  </si>
+  <si>
+    <t>IPA07</t>
+  </si>
+  <si>
+    <t>OPQA-4387||OPQA-4372||OPQA-4373||OPQA-4374||OPQA-4376||OPQA-4377||OPQA-4378||OPQA-4379</t>
+  </si>
+  <si>
+    <t>Verify Mandatory Field and Sorting with Different options at Technology ResultList</t>
+  </si>
+  <si>
+    <t>IPA08</t>
+  </si>
+  <si>
+    <t>OPQA-4387||OPQA-4380||OPQA-4381||OPQA-4384||OPQA-4385||OPQA-4386</t>
+  </si>
+  <si>
+    <t>Verify Mandatory Field and Sorting with Different options at Company ResultList</t>
   </si>
 </sst>
 </file>
@@ -360,19 +426,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -703,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E29"/>
+      <selection activeCell="A31" sqref="A1:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1089,87 +1147,87 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="120">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="255">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="150">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="D29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1187,6 +1245,126 @@
         <v>5</v>
       </c>
       <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
fixed test scripts in IPA module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -365,12 +365,23 @@
   <si>
     <t>Verify Mandatory Field and Sorting with Different options at Company ResultList</t>
   </si>
+  <si>
+    <t>OPQA-4447,OPQA-4448,OPQA-4454,OPQA-4455,OPQA-4460,OPQA-4479,OPQA-4480,OPQA-4481,OPQA-4483</t>
+  </si>
+  <si>
+    <t>OPQA-4466,OPQA-4467, OPQA-4468,OPQA-4471,OPQA-4474,OPQA-4475,OPQA-4476,OPQA-4477,OPQA-4486</t>
+  </si>
+  <si>
+    <t>OPQA-4455,OPQA-4457,OPQA-4461,OPQA-4462</t>
+  </si>
+  <si>
+    <t>OPQA-4464,OPQA-4478</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -764,17 +775,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A31" sqref="A1:E38"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="63.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="63" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -799,7 +810,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -816,7 +827,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -1137,7 +1148,7 @@
         <v>71</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>11</v>
@@ -1252,7 +1263,7 @@
         <v>89</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
modified test cases in IPA module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="15576" windowHeight="6216"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15570" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t>TCID</t>
   </si>
@@ -48,12 +48,6 @@
     <t>IPA111</t>
   </si>
   <si>
-    <t>Save the company search data and rerun the saved data</t>
-  </si>
-  <si>
-    <t>Save the technology search data and rerun the saved data</t>
-  </si>
-  <si>
     <t>NEON-291||NEON-400||NEON-438||NEON-574</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>IPA112</t>
-  </si>
-  <si>
     <t>IPA5</t>
   </si>
   <si>
@@ -79,9 +70,6 @@
   </si>
   <si>
     <t>OPQA-4197||OPQA-4199||OPQA-4215||OPQA-4216||OPQA-4201</t>
-  </si>
-  <si>
-    <t>Verify that profile fly-out will display profile meta-data||Verify that profile fly-out provides access to the profile modal.||Verify that the profile fly-out should display the following user profile details, if available: a)First name b)Last Name c)Title d)Institution e)Country f)Photo||Verify that by clicking on any of the following fields (when present), will provide access to the profile modal. 1.Name 2.Institution 3. Country 4 .Title 5.Photo || Verify that profile fly-out provides access to the account setting modal</t>
   </si>
   <si>
     <t>Verify that the profile fly-out should contain link to terms of use||Verify that profile fly-out should contain link to privacy statement||Verify that the profile fly-out should contain link to app-specific feedback page||Verify that the profile fly-out should contain link to app-specific help page||Verify that the alternative profile fly-out should contain link to sign out of the platform. User returns to sign-in page.</t>
@@ -219,18 +207,6 @@
   </si>
   <si>
     <t>Verify Mandatory Field and Sorting with Different options at Company ResultList</t>
-  </si>
-  <si>
-    <t>OPQA-4447,OPQA-4448,OPQA-4454,OPQA-4455,OPQA-4460,OPQA-4479,OPQA-4480,OPQA-4481,OPQA-4483</t>
-  </si>
-  <si>
-    <t>OPQA-4466,OPQA-4467, OPQA-4468,OPQA-4471,OPQA-4474,OPQA-4475,OPQA-4476,OPQA-4477,OPQA-4486</t>
-  </si>
-  <si>
-    <t>OPQA-4455,OPQA-4457,OPQA-4461,OPQA-4462</t>
-  </si>
-  <si>
-    <t>OPQA-4464,OPQA-4478</t>
   </si>
   <si>
     <t>OPQA-1934||
@@ -245,10 +221,40 @@
 OPQA-4252</t>
   </si>
   <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
-  </si>
-  <si>
     <t>IPA100</t>
+  </si>
+  <si>
+    <t>OPQA-4447||OPQA-4448||OPQA-4454||OPQA-4455||OPQA-4460||OPQA-4479||OPQA-4480||OPQA-4481||OPQA-4483</t>
+  </si>
+  <si>
+    <t>OPQA-4466||OPQA-4467|| OPQA-4468||OPQA-4471||OPQA-4474||OPQA-4475||OPQA-4476||OPQA-4477||OPQA-4486</t>
+  </si>
+  <si>
+    <t>Verify that profile fly-out will display profile meta-data||Verify that profile fly-out provides access to the profile modal.||Verify that the profile fly-out should display the following user profile details|| if available: a)First name b)Last Name c)Title d)Institution e)Country f)Photo||Verify that by clicking on any of the following fields (when present)|| will provide access to the profile modal. 1.Name 2.Institution 3. Country 4 .Title 5.Photo || Verify that profile fly-out provides access to the account setting modal</t>
+  </si>
+  <si>
+    <t>OPQA-4464||OPQA-4478</t>
+  </si>
+  <si>
+    <t>OPQA-4455||OPQA-4457||OPQA-4461||OPQA-4462</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not|| after clicking on Forgot your password? Link&amp;Verify that||the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid|| upon clicking the password reset link in the the platform forget password email|| the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change|| The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used|| upon clicking the password reset link in the the platform forget password email|| the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page|| should be taken to the target application sign in page.||Verify that when Email address is known from password reset token||error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token||email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sort the saved search by applying sort options as  Date saved and Date viewed</t>
+  </si>
+  <si>
+    <t>Verify that user is able to perform technology search and Save search data and rerun the saved data and verify that all values are dispalying for the saved search</t>
+  </si>
+  <si>
+    <t>Verify that user is able to perform Company search and Save search data and rerun the saved data and verify that all values are dispalying for the saved search</t>
+  </si>
+  <si>
+    <t>Verify that user is able to navigate to record view page of patents and verify all options are displaying or not</t>
+  </si>
+  <si>
+    <t>Verify that user is able to save data without description and user is able to edit the saved data title and desc and able to delete selected saved data tile</t>
   </si>
 </sst>
 </file>
@@ -664,19 +670,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="63" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -701,10 +707,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -718,10 +724,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -732,85 +738,85 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="105">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="120">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="86.4">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="120">
+      <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="100.8">
-      <c r="A7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="115.2">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="255">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -823,238 +829,221 @@
         <v>5</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="150">
+      <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="216">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="144">
-      <c r="A11" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.8">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="B14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="D17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="D18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="D20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="D21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="270">
       <c r="A22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>62</v>
+      <c r="B22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="216">
-      <c r="A23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="4"/>
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1067,7 +1056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1079,7 +1068,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed ipa100 from IPA suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="15570" windowHeight="6210"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>TCID</t>
   </si>
@@ -209,21 +214,6 @@
     <t>Verify Mandatory Field and Sorting with Different options at Company ResultList</t>
   </si>
   <si>
-    <t>OPQA-1934||
-OPQA-1935&amp;OPQA-3687||
-OPQA-4230||OPQA-4229||
-OPQA-4231||OPQA-4232||
-OPQA-4636||OPQA-4261||
-OPQA-4244||OPQA-4264||
-OPQA-4265||OPQA-4237||
-OPQA-4239||OPQA-4240||
-OPQA-4246||OPQA-4248||
-OPQA-4252</t>
-  </si>
-  <si>
-    <t>IPA100</t>
-  </si>
-  <si>
     <t>OPQA-4447||OPQA-4448||OPQA-4454||OPQA-4455||OPQA-4460||OPQA-4479||OPQA-4480||OPQA-4481||OPQA-4483</t>
   </si>
   <si>
@@ -237,9 +227,6 @@
   </si>
   <si>
     <t>OPQA-4455||OPQA-4457||OPQA-4461||OPQA-4462</t>
-  </si>
-  <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not|| after clicking on Forgot your password? Link&amp;Verify that||the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid|| upon clicking the password reset link in the the platform forget password email|| the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change|| The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used|| upon clicking the password reset link in the the platform forget password email|| the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page|| should be taken to the target application sign in page.||Verify that when Email address is known from password reset token||error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token||email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
   </si>
   <si>
     <t>Verify that user is able to sort the saved search by applying sort options as  Date saved and Date viewed</t>
@@ -260,8 +247,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,9 +447,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,6 +482,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,14 +658,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -685,7 +674,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,15 +691,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -719,15 +708,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -736,7 +725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -753,7 +742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="105">
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -768,7 +757,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="120">
+    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -776,29 +765,29 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="120">
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -815,7 +804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="255">
+    <row r="9" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -832,7 +821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150">
+    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
@@ -849,7 +838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -866,7 +855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
@@ -883,7 +872,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -891,29 +880,29 @@
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
@@ -930,7 +919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>41</v>
       </c>
@@ -947,7 +936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
@@ -964,7 +953,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -981,7 +970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>50</v>
       </c>
@@ -998,7 +987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>53</v>
       </c>
@@ -1013,7 +1002,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>56</v>
       </c>
@@ -1030,19 +1019,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="270">
-      <c r="A22" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>5</v>
-      </c>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
   </sheetData>
@@ -1051,24 +1032,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified the script names with proper standard for IPA
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1p-projects\Latest\1p-ui-automation\src\test\resources\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>TCID</t>
   </si>
@@ -38,39 +38,21 @@
     <t>Results</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>SKIP</t>
   </si>
   <si>
     <t>OBT</t>
   </si>
   <si>
-    <t>IPA001</t>
-  </si>
-  <si>
-    <t>IPA111</t>
-  </si>
-  <si>
     <t>NEON-291||NEON-400||NEON-438||NEON-574</t>
   </si>
   <si>
     <t>User must be able to form a Technology Search||User must be able to return to the app landing page via the App header to start a new search||Option on the IPA App header to allow the user to return to the app landing page||User must be able to form a Company Search</t>
   </si>
   <si>
-    <t>IPA012</t>
-  </si>
-  <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t>IPA5</t>
-  </si>
-  <si>
-    <t>IPA6</t>
-  </si>
-  <si>
     <t>OPQA-4205||OPQA-4207||OPQA-4208||OPQA-4210||OPQA-4211</t>
   </si>
   <si>
@@ -78,9 +60,6 @@
   </si>
   <si>
     <t>Verify that the profile fly-out should contain link to terms of use||Verify that profile fly-out should contain link to privacy statement||Verify that the profile fly-out should contain link to app-specific feedback page||Verify that the profile fly-out should contain link to app-specific help page||Verify that the alternative profile fly-out should contain link to sign out of the platform. User returns to sign-in page.</t>
-  </si>
-  <si>
-    <t>IPA113</t>
   </si>
   <si>
     <t>IPA10</t>
@@ -139,18 +118,12 @@
     <t>IPA14</t>
   </si>
   <si>
-    <t>IPA114</t>
-  </si>
-  <si>
     <t>OPQA-4389||OPQA-4390</t>
   </si>
   <si>
     <t>User must be able to select to record on the result list to view its full content</t>
   </si>
   <si>
-    <t>IPA115</t>
-  </si>
-  <si>
     <t>IPA02</t>
   </si>
   <si>
@@ -242,6 +215,42 @@
   </si>
   <si>
     <t>Verify that user is able to save data without description and user is able to edit the saved data title and desc and able to delete selected saved data tile</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>IPA01</t>
+  </si>
+  <si>
+    <t>IPA09</t>
+  </si>
+  <si>
+    <t>IPA15</t>
+  </si>
+  <si>
+    <t>IPA17</t>
+  </si>
+  <si>
+    <t>IPA18</t>
+  </si>
+  <si>
+    <t>IPA19</t>
+  </si>
+  <si>
+    <t>IPA20</t>
+  </si>
+  <si>
+    <t>IPA21</t>
+  </si>
+  <si>
+    <t>IPA16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View By </t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -311,20 +320,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -659,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,357 +684,373 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="B19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="255" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="C22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="D22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1035,7 +1061,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Adding two new scripts IPA22 and IPA23
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
   <si>
     <t>TCID</t>
   </si>
@@ -252,22 +252,36 @@
   <si>
     <t>View By test cases</t>
   </si>
+  <si>
+    <t>IPA22</t>
+  </si>
+  <si>
+    <t>IPA23</t>
+  </si>
+  <si>
+    <t>OPQA-4853||OPQA-4854||OPQA-4856</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that system provides pin option to visualization tabs when user visits dashboard Page|| Verify that system doesn't provides pin option for patents tab when user visits dashboard Page|| Verify that system dispalys all visualization when user selects pin option in every  visualizations tabs</t>
+  </si>
+  <si>
+    <t>OPQA-4900||OPQA-4901||OPQA-4902</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that system provides pin option to visualization tabs when user visits dashboard Page|| Verify that system doesn't provides pin option for patents tab when user visits dashboard Page|| Verify that system dispalys all visualization when user select</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,15 +334,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -671,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,36 +696,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -728,8 +739,8 @@
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>60</v>
+      <c r="D3" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -745,8 +756,8 @@
       <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>60</v>
+      <c r="D4" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -762,8 +773,8 @@
       <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>60</v>
+      <c r="D5" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -779,8 +790,8 @@
       <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>60</v>
+      <c r="D6" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -796,8 +807,8 @@
       <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>60</v>
+      <c r="D7" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -813,8 +824,8 @@
       <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>60</v>
+      <c r="D8" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -828,8 +839,8 @@
       <c r="C9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>60</v>
+      <c r="D9" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
@@ -845,8 +856,8 @@
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>60</v>
+      <c r="D10" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
@@ -862,8 +873,8 @@
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>60</v>
+      <c r="D11" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -879,8 +890,8 @@
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>60</v>
+      <c r="D12" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -896,8 +907,8 @@
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>60</v>
+      <c r="D13" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -913,8 +924,8 @@
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>60</v>
+      <c r="D14" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -930,8 +941,8 @@
       <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>60</v>
+      <c r="D15" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -947,8 +958,8 @@
       <c r="C16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>60</v>
+      <c r="D16" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -962,8 +973,8 @@
       <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>60</v>
+      <c r="D17" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -977,27 +988,27 @@
       <c r="C18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>60</v>
+      <c r="D18" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="5"/>
+      <c r="D19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1009,8 +1020,8 @@
       <c r="C20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>60</v>
+      <c r="D20" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1024,8 +1035,8 @@
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>60</v>
+      <c r="D21" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1039,20 +1050,40 @@
       <c r="C22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="5"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating the new scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/IPA.xlsx
+++ b/src/test/resources/xls/IPA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>TCID</t>
   </si>
@@ -269,9 +269,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Verify that system provides pin option to visualization tabs when user visits dashboard Page|| Verify that system doesn't provides pin option for patents tab when user visits dashboard Page|| Verify that system dispalys all visualization when user select</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -683,7 +680,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D2" sqref="D2:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +720,7 @@
         <v>56</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -740,7 +737,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -757,7 +754,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -774,7 +771,7 @@
         <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -791,7 +788,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -808,7 +805,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -825,7 +822,7 @@
         <v>46</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -840,7 +837,7 @@
         <v>49</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
@@ -857,7 +854,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
@@ -874,7 +871,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -891,7 +888,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -908,7 +905,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -925,7 +922,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -942,7 +939,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -959,7 +956,7 @@
         <v>59</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -974,7 +971,7 @@
         <v>71</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -989,7 +986,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -1006,7 +1003,7 @@
         <v>55</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E19" s="4"/>
     </row>
@@ -1021,7 +1018,7 @@
         <v>58</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1036,7 +1033,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1051,7 +1048,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1"/>
     </row>

</xml_diff>